<commit_message>
Added docx reader/writer feature
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Roll No.</t>
   </si>
@@ -35,6 +35,18 @@
   </si>
   <si>
     <t xml:space="preserve">Attendance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arun Nair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appuarunnair@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rajeswary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">janeswarynair@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -44,7 +56,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -69,6 +81,13 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -116,12 +135,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -142,19 +169,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.4540816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6326530612245"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
@@ -175,7 +202,45 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>9820055038</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>7718055035</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="appuarunnair@gmail.com"/>
+    <hyperlink ref="C3" r:id="rId2" display="janeswarynair@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>